<commit_message>
Modified config.py and rebuild.py to make use of the HAZUS repair times lookup table
</commit_message>
<xml_diff>
--- a/inputs/hazus_parameters.xlsx
+++ b/inputs/hazus_parameters.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="680" yWindow="940" windowWidth="27360" windowHeight="15820" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="680" yWindow="940" windowWidth="27360" windowHeight="15820" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Struct. Repair Cost % of value" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="117">
   <si>
     <t>No.</t>
   </si>
@@ -419,7 +419,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -427,6 +427,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2253,8 +2254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2299,8 +2300,8 @@
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>116</v>
+      <c r="D2" s="5">
+        <v>0</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
@@ -2325,8 +2326,8 @@
       <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>116</v>
+      <c r="D3" s="5">
+        <v>0</v>
       </c>
       <c r="E3" s="1">
         <v>0.8</v>
@@ -2351,8 +2352,8 @@
       <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>116</v>
+      <c r="D4" s="5">
+        <v>0</v>
       </c>
       <c r="E4" s="1">
         <v>0.9</v>
@@ -2377,8 +2378,8 @@
       <c r="C5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>116</v>
+      <c r="D5" s="5">
+        <v>0</v>
       </c>
       <c r="E5" s="1">
         <v>0.9</v>
@@ -2403,8 +2404,8 @@
       <c r="C6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>116</v>
+      <c r="D6" s="5">
+        <v>0</v>
       </c>
       <c r="E6" s="1">
         <v>0.8</v>
@@ -2429,8 +2430,8 @@
       <c r="C7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>116</v>
+      <c r="D7" s="5">
+        <v>0</v>
       </c>
       <c r="E7" s="1">
         <v>0.8</v>
@@ -2455,8 +2456,8 @@
       <c r="C8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>116</v>
+      <c r="D8" s="5">
+        <v>0</v>
       </c>
       <c r="E8" s="1">
         <v>0.6</v>
@@ -2481,8 +2482,8 @@
       <c r="C9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>116</v>
+      <c r="D9" s="5">
+        <v>0</v>
       </c>
       <c r="E9" s="1">
         <v>0.6</v>
@@ -2507,8 +2508,8 @@
       <c r="C10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>116</v>
+      <c r="D10" s="5">
+        <v>0</v>
       </c>
       <c r="E10" s="1">
         <v>0.7</v>
@@ -2533,8 +2534,8 @@
       <c r="C11" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>116</v>
+      <c r="D11" s="5">
+        <v>0</v>
       </c>
       <c r="E11" s="1">
         <v>0.7</v>
@@ -2559,8 +2560,8 @@
       <c r="C12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>116</v>
+      <c r="D12" s="5">
+        <v>0</v>
       </c>
       <c r="E12" s="1">
         <v>0.7</v>
@@ -2585,8 +2586,8 @@
       <c r="C13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>116</v>
+      <c r="D13" s="5">
+        <v>0</v>
       </c>
       <c r="E13" s="1">
         <v>0.8</v>
@@ -2611,8 +2612,8 @@
       <c r="C14" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>116</v>
+      <c r="D14" s="5">
+        <v>0</v>
       </c>
       <c r="E14" s="1">
         <v>0.7</v>
@@ -2637,8 +2638,8 @@
       <c r="C15" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>116</v>
+      <c r="D15" s="5">
+        <v>0</v>
       </c>
       <c r="E15" s="1">
         <v>0.7</v>
@@ -2663,8 +2664,8 @@
       <c r="C16" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>116</v>
+      <c r="D16" s="5">
+        <v>0</v>
       </c>
       <c r="E16" s="1">
         <v>0.7</v>
@@ -2689,8 +2690,8 @@
       <c r="C17" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>116</v>
+      <c r="D17" s="5">
+        <v>0</v>
       </c>
       <c r="E17" s="1">
         <v>0.4</v>
@@ -2715,8 +2716,8 @@
       <c r="C18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>116</v>
+      <c r="D18" s="5">
+        <v>0</v>
       </c>
       <c r="E18" s="1">
         <v>0.2</v>
@@ -2741,8 +2742,8 @@
       <c r="C19" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>116</v>
+      <c r="D19" s="5">
+        <v>0</v>
       </c>
       <c r="E19" s="1">
         <v>0.2</v>
@@ -2767,8 +2768,8 @@
       <c r="C20" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>116</v>
+      <c r="D20" s="5">
+        <v>0</v>
       </c>
       <c r="E20" s="1">
         <v>0.2</v>
@@ -2793,8 +2794,8 @@
       <c r="C21" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>116</v>
+      <c r="D21" s="5">
+        <v>0</v>
       </c>
       <c r="E21" s="1">
         <v>0.2</v>
@@ -2819,8 +2820,8 @@
       <c r="C22" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="4" t="s">
-        <v>116</v>
+      <c r="D22" s="5">
+        <v>0</v>
       </c>
       <c r="E22" s="1">
         <v>0.2</v>
@@ -2845,8 +2846,8 @@
       <c r="C23" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D23" s="4" t="s">
-        <v>116</v>
+      <c r="D23" s="5">
+        <v>0</v>
       </c>
       <c r="E23" s="1">
         <v>0.2</v>
@@ -2871,8 +2872,8 @@
       <c r="C24" t="s">
         <v>50</v>
       </c>
-      <c r="D24" s="4" t="s">
-        <v>116</v>
+      <c r="D24" s="5">
+        <v>0</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -2897,8 +2898,8 @@
       <c r="C25" t="s">
         <v>91</v>
       </c>
-      <c r="D25" s="4" t="s">
-        <v>116</v>
+      <c r="D25" s="5">
+        <v>0</v>
       </c>
       <c r="E25">
         <v>0.8</v>
@@ -2923,8 +2924,8 @@
       <c r="C26" t="s">
         <v>55</v>
       </c>
-      <c r="D26" s="4" t="s">
-        <v>116</v>
+      <c r="D26" s="5">
+        <v>0</v>
       </c>
       <c r="E26">
         <v>0.7</v>
@@ -2949,8 +2950,8 @@
       <c r="C27" t="s">
         <v>57</v>
       </c>
-      <c r="D27" s="4" t="s">
-        <v>116</v>
+      <c r="D27" s="5">
+        <v>0</v>
       </c>
       <c r="E27">
         <v>0.7</v>
@@ -2975,8 +2976,8 @@
       <c r="C28" t="s">
         <v>59</v>
       </c>
-      <c r="D28" s="4" t="s">
-        <v>116</v>
+      <c r="D28" s="5">
+        <v>0</v>
       </c>
       <c r="E28">
         <v>0.9</v>
@@ -3001,8 +3002,8 @@
       <c r="C29" t="s">
         <v>61</v>
       </c>
-      <c r="D29" s="4" t="s">
-        <v>116</v>
+      <c r="D29" s="5">
+        <v>0</v>
       </c>
       <c r="E29">
         <v>1.2</v>
@@ -3026,8 +3027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>